<commit_message>
Update Pico Dsiplay Pixel Map.xlsx
</commit_message>
<xml_diff>
--- a/Pico Dsiplay Pixel Map.xlsx
+++ b/Pico Dsiplay Pixel Map.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/816ce93561dbac4d/RPi Projects/Pico/playing-with-pico/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="108" documentId="8_{95987369-0CCB-4E7E-9497-FD5820FBA44B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DC2EF6D4-3E0E-4A09-88D1-DE900108B071}"/>
+  <xr:revisionPtr revIDLastSave="189" documentId="8_{95987369-0CCB-4E7E-9497-FD5820FBA44B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{10F3CBCF-AB79-4208-8139-8E18C687BF2F}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{61589EE4-630A-4E32-9F01-8BE1ECA5321B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{61589EE4-630A-4E32-9F01-8BE1ECA5321B}"/>
   </bookViews>
   <sheets>
     <sheet name="Pico Display Map" sheetId="1" r:id="rId1"/>
     <sheet name="Scroll Map" sheetId="2" r:id="rId2"/>
+    <sheet name="Tetris Shapes" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Pico Display Map'!$A$1:$EF$241</definedName>
@@ -39,9 +40,44 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+  <si>
+    <t>O_Block</t>
+  </si>
+  <si>
+    <t>Position 1</t>
+  </si>
+  <si>
+    <t>Position 2</t>
+  </si>
+  <si>
+    <t>Position 3</t>
+  </si>
+  <si>
+    <t>Position 4</t>
+  </si>
+  <si>
+    <t>I_Block</t>
+  </si>
+  <si>
+    <t>J_Block</t>
+  </si>
+  <si>
+    <t>S_Block</t>
+  </si>
+  <si>
+    <t>Z_Block</t>
+  </si>
+  <si>
+    <t>T_Block</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -63,8 +99,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -82,8 +124,50 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="18">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -326,12 +410,129 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -362,22 +563,73 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="3">
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <font>
         <color auto="1"/>
@@ -395,6 +647,16 @@
       <fill>
         <patternFill>
           <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -34744,7 +35006,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9E7EBA5-D2E2-4ECF-BBC7-F4FE26419266}">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
@@ -35220,17 +35482,1276 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:H18">
-    <cfRule type="expression" dxfId="2" priority="2">
+    <cfRule type="expression" dxfId="2" priority="1">
+      <formula>NOT(OR(B2=1,B2=0))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>B2=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="3">
+    <cfRule type="expression" dxfId="0" priority="3">
       <formula>B2 =1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="0" priority="1">
-      <formula>NOT(OR(B2=1,B2=0))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63E2095A-F482-4ED0-A8EE-549022EB1492}">
+  <dimension ref="A1:Z43"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="AH10" sqref="AH10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="30" width="3.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="43"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="43" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" s="44"/>
+      <c r="K1" s="44"/>
+      <c r="L1" s="44"/>
+      <c r="M1" s="44"/>
+      <c r="N1" s="45"/>
+      <c r="O1" s="43" t="s">
+        <v>3</v>
+      </c>
+      <c r="P1" s="44"/>
+      <c r="Q1" s="44"/>
+      <c r="R1" s="44"/>
+      <c r="S1" s="44"/>
+      <c r="T1" s="45"/>
+      <c r="U1" s="43" t="s">
+        <v>4</v>
+      </c>
+      <c r="V1" s="44"/>
+      <c r="W1" s="44"/>
+      <c r="X1" s="44"/>
+      <c r="Y1" s="44"/>
+      <c r="Z1" s="45"/>
+    </row>
+    <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="51"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="48"/>
+      <c r="J2" s="50"/>
+      <c r="K2" s="50"/>
+      <c r="L2" s="50"/>
+      <c r="M2" s="50"/>
+      <c r="N2" s="49"/>
+      <c r="O2" s="48"/>
+      <c r="P2" s="50"/>
+      <c r="Q2" s="50"/>
+      <c r="R2" s="50"/>
+      <c r="S2" s="50"/>
+      <c r="T2" s="49"/>
+      <c r="U2" s="48"/>
+      <c r="V2" s="50"/>
+      <c r="W2" s="50"/>
+      <c r="X2" s="50"/>
+      <c r="Y2" s="50"/>
+      <c r="Z2" s="49"/>
+    </row>
+    <row r="3" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="32"/>
+      <c r="B3" s="46"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="40"/>
+      <c r="J3" s="34"/>
+      <c r="K3" s="34"/>
+      <c r="L3" s="34"/>
+      <c r="M3" s="34"/>
+      <c r="N3" s="35"/>
+      <c r="O3" s="40"/>
+      <c r="P3" s="34"/>
+      <c r="Q3" s="34"/>
+      <c r="R3" s="34"/>
+      <c r="S3" s="34"/>
+      <c r="T3" s="35"/>
+      <c r="U3" s="40"/>
+      <c r="V3" s="34"/>
+      <c r="W3" s="34"/>
+      <c r="X3" s="34"/>
+      <c r="Y3" s="34"/>
+      <c r="Z3" s="35"/>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A4" s="32"/>
+      <c r="B4" s="46"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="34"/>
+      <c r="H4" s="35"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="34"/>
+      <c r="K4" s="24"/>
+      <c r="L4" s="24"/>
+      <c r="M4" s="34"/>
+      <c r="N4" s="35"/>
+      <c r="O4" s="40"/>
+      <c r="P4" s="34"/>
+      <c r="Q4" s="24"/>
+      <c r="R4" s="24"/>
+      <c r="S4" s="34"/>
+      <c r="T4" s="35"/>
+      <c r="U4" s="40"/>
+      <c r="V4" s="34"/>
+      <c r="W4" s="24"/>
+      <c r="X4" s="24"/>
+      <c r="Y4" s="34"/>
+      <c r="Z4" s="35"/>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A5" s="32"/>
+      <c r="B5" s="46"/>
+      <c r="C5" s="40"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="35"/>
+      <c r="I5" s="40"/>
+      <c r="J5" s="34"/>
+      <c r="K5" s="24"/>
+      <c r="L5" s="24"/>
+      <c r="M5" s="34"/>
+      <c r="N5" s="35"/>
+      <c r="O5" s="40"/>
+      <c r="P5" s="34"/>
+      <c r="Q5" s="24"/>
+      <c r="R5" s="24"/>
+      <c r="S5" s="34"/>
+      <c r="T5" s="35"/>
+      <c r="U5" s="40"/>
+      <c r="V5" s="34"/>
+      <c r="W5" s="24"/>
+      <c r="X5" s="24"/>
+      <c r="Y5" s="34"/>
+      <c r="Z5" s="35"/>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A6" s="32"/>
+      <c r="B6" s="46"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="34"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="35"/>
+      <c r="I6" s="40"/>
+      <c r="J6" s="34"/>
+      <c r="K6" s="34"/>
+      <c r="L6" s="34"/>
+      <c r="M6" s="34"/>
+      <c r="N6" s="35"/>
+      <c r="O6" s="40"/>
+      <c r="P6" s="34"/>
+      <c r="Q6" s="34"/>
+      <c r="R6" s="34"/>
+      <c r="S6" s="34"/>
+      <c r="T6" s="35"/>
+      <c r="U6" s="40"/>
+      <c r="V6" s="34"/>
+      <c r="W6" s="34"/>
+      <c r="X6" s="34"/>
+      <c r="Y6" s="34"/>
+      <c r="Z6" s="35"/>
+    </row>
+    <row r="7" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="36"/>
+      <c r="B7" s="47"/>
+      <c r="C7" s="41"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="38"/>
+      <c r="G7" s="38"/>
+      <c r="H7" s="39"/>
+      <c r="I7" s="41"/>
+      <c r="J7" s="38"/>
+      <c r="K7" s="38"/>
+      <c r="L7" s="38"/>
+      <c r="M7" s="38"/>
+      <c r="N7" s="39"/>
+      <c r="O7" s="41"/>
+      <c r="P7" s="38"/>
+      <c r="Q7" s="38"/>
+      <c r="R7" s="38"/>
+      <c r="S7" s="38"/>
+      <c r="T7" s="39"/>
+      <c r="U7" s="41"/>
+      <c r="V7" s="38"/>
+      <c r="W7" s="38"/>
+      <c r="X7" s="38"/>
+      <c r="Y7" s="38"/>
+      <c r="Z7" s="39"/>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A8" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="29"/>
+      <c r="C8" s="42"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="30"/>
+      <c r="H8" s="31"/>
+      <c r="I8" s="42"/>
+      <c r="J8" s="30"/>
+      <c r="K8" s="30"/>
+      <c r="L8" s="30"/>
+      <c r="M8" s="30"/>
+      <c r="N8" s="31"/>
+      <c r="O8" s="42"/>
+      <c r="P8" s="30"/>
+      <c r="Q8" s="30"/>
+      <c r="R8" s="30"/>
+      <c r="S8" s="30"/>
+      <c r="T8" s="31"/>
+      <c r="U8" s="42"/>
+      <c r="V8" s="30"/>
+      <c r="W8" s="30"/>
+      <c r="X8" s="30"/>
+      <c r="Y8" s="30"/>
+      <c r="Z8" s="31"/>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A9" s="32"/>
+      <c r="B9" s="33"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="34"/>
+      <c r="E9" s="34"/>
+      <c r="F9" s="34"/>
+      <c r="G9" s="34"/>
+      <c r="H9" s="35"/>
+      <c r="I9" s="40"/>
+      <c r="J9" s="34"/>
+      <c r="K9" s="25"/>
+      <c r="L9" s="34"/>
+      <c r="M9" s="34"/>
+      <c r="N9" s="35"/>
+      <c r="O9" s="40"/>
+      <c r="P9" s="34"/>
+      <c r="Q9" s="34"/>
+      <c r="R9" s="34"/>
+      <c r="S9" s="34"/>
+      <c r="T9" s="35"/>
+      <c r="U9" s="40"/>
+      <c r="V9" s="34"/>
+      <c r="W9" s="34"/>
+      <c r="X9" s="25"/>
+      <c r="Y9" s="34"/>
+      <c r="Z9" s="35"/>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A10" s="32"/>
+      <c r="B10" s="33"/>
+      <c r="C10" s="40"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="25"/>
+      <c r="H10" s="35"/>
+      <c r="I10" s="40"/>
+      <c r="J10" s="34"/>
+      <c r="K10" s="25"/>
+      <c r="L10" s="34"/>
+      <c r="M10" s="34"/>
+      <c r="N10" s="35"/>
+      <c r="O10" s="40"/>
+      <c r="P10" s="25"/>
+      <c r="Q10" s="25"/>
+      <c r="R10" s="25"/>
+      <c r="S10" s="25"/>
+      <c r="T10" s="35"/>
+      <c r="U10" s="40"/>
+      <c r="V10" s="34"/>
+      <c r="W10" s="34"/>
+      <c r="X10" s="25"/>
+      <c r="Y10" s="34"/>
+      <c r="Z10" s="35"/>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A11" s="32"/>
+      <c r="B11" s="33"/>
+      <c r="C11" s="40"/>
+      <c r="D11" s="34"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
+      <c r="G11" s="34"/>
+      <c r="H11" s="35"/>
+      <c r="I11" s="40"/>
+      <c r="J11" s="34"/>
+      <c r="K11" s="25"/>
+      <c r="L11" s="34"/>
+      <c r="M11" s="34"/>
+      <c r="N11" s="35"/>
+      <c r="O11" s="40"/>
+      <c r="P11" s="34"/>
+      <c r="Q11" s="34"/>
+      <c r="R11" s="34"/>
+      <c r="S11" s="34"/>
+      <c r="T11" s="35"/>
+      <c r="U11" s="40"/>
+      <c r="V11" s="34"/>
+      <c r="W11" s="34"/>
+      <c r="X11" s="25"/>
+      <c r="Y11" s="34"/>
+      <c r="Z11" s="35"/>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A12" s="32"/>
+      <c r="B12" s="33"/>
+      <c r="C12" s="40"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="34"/>
+      <c r="H12" s="35"/>
+      <c r="I12" s="40"/>
+      <c r="J12" s="34"/>
+      <c r="K12" s="25"/>
+      <c r="L12" s="34"/>
+      <c r="M12" s="34"/>
+      <c r="N12" s="35"/>
+      <c r="O12" s="40"/>
+      <c r="P12" s="34"/>
+      <c r="Q12" s="34"/>
+      <c r="R12" s="34"/>
+      <c r="S12" s="34"/>
+      <c r="T12" s="35"/>
+      <c r="U12" s="40"/>
+      <c r="V12" s="34"/>
+      <c r="W12" s="34"/>
+      <c r="X12" s="25"/>
+      <c r="Y12" s="34"/>
+      <c r="Z12" s="35"/>
+    </row>
+    <row r="13" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="36"/>
+      <c r="B13" s="37"/>
+      <c r="C13" s="41"/>
+      <c r="D13" s="38"/>
+      <c r="E13" s="38"/>
+      <c r="F13" s="38"/>
+      <c r="G13" s="38"/>
+      <c r="H13" s="39"/>
+      <c r="I13" s="41"/>
+      <c r="J13" s="38"/>
+      <c r="K13" s="38"/>
+      <c r="L13" s="38"/>
+      <c r="M13" s="38"/>
+      <c r="N13" s="39"/>
+      <c r="O13" s="41"/>
+      <c r="P13" s="38"/>
+      <c r="Q13" s="38"/>
+      <c r="R13" s="38"/>
+      <c r="S13" s="38"/>
+      <c r="T13" s="39"/>
+      <c r="U13" s="41"/>
+      <c r="V13" s="38"/>
+      <c r="W13" s="38"/>
+      <c r="X13" s="38"/>
+      <c r="Y13" s="38"/>
+      <c r="Z13" s="39"/>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A14" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="29"/>
+      <c r="C14" s="42"/>
+      <c r="D14" s="30"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="30"/>
+      <c r="H14" s="31"/>
+      <c r="I14" s="42"/>
+      <c r="J14" s="30"/>
+      <c r="K14" s="30"/>
+      <c r="L14" s="30"/>
+      <c r="M14" s="30"/>
+      <c r="N14" s="31"/>
+      <c r="O14" s="42"/>
+      <c r="P14" s="30"/>
+      <c r="Q14" s="30"/>
+      <c r="R14" s="30"/>
+      <c r="S14" s="30"/>
+      <c r="T14" s="31"/>
+      <c r="U14" s="42"/>
+      <c r="V14" s="30"/>
+      <c r="W14" s="30"/>
+      <c r="X14" s="30"/>
+      <c r="Y14" s="30"/>
+      <c r="Z14" s="31"/>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A15" s="32"/>
+      <c r="B15" s="33"/>
+      <c r="C15" s="40"/>
+      <c r="D15" s="34"/>
+      <c r="E15" s="34"/>
+      <c r="F15" s="34"/>
+      <c r="G15" s="34"/>
+      <c r="H15" s="35"/>
+      <c r="I15" s="40"/>
+      <c r="J15" s="34"/>
+      <c r="K15" s="34"/>
+      <c r="L15" s="34"/>
+      <c r="M15" s="34"/>
+      <c r="N15" s="35"/>
+      <c r="O15" s="40"/>
+      <c r="P15" s="34"/>
+      <c r="Q15" s="34"/>
+      <c r="R15" s="34"/>
+      <c r="S15" s="34"/>
+      <c r="T15" s="35"/>
+      <c r="U15" s="40"/>
+      <c r="V15" s="34"/>
+      <c r="W15" s="34"/>
+      <c r="X15" s="34"/>
+      <c r="Y15" s="34"/>
+      <c r="Z15" s="35"/>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A16" s="32"/>
+      <c r="B16" s="33"/>
+      <c r="C16" s="40"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="34"/>
+      <c r="F16" s="34"/>
+      <c r="G16" s="34"/>
+      <c r="H16" s="35"/>
+      <c r="I16" s="40"/>
+      <c r="J16" s="34"/>
+      <c r="K16" s="26"/>
+      <c r="L16" s="26"/>
+      <c r="M16" s="34"/>
+      <c r="N16" s="35"/>
+      <c r="O16" s="40"/>
+      <c r="P16" s="34"/>
+      <c r="Q16" s="26"/>
+      <c r="R16" s="26"/>
+      <c r="S16" s="26"/>
+      <c r="T16" s="35"/>
+      <c r="U16" s="40"/>
+      <c r="V16" s="34"/>
+      <c r="W16" s="34"/>
+      <c r="X16" s="26"/>
+      <c r="Y16" s="34"/>
+      <c r="Z16" s="35"/>
+    </row>
+    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A17" s="32"/>
+      <c r="B17" s="33"/>
+      <c r="C17" s="40"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="26"/>
+      <c r="F17" s="26"/>
+      <c r="G17" s="34"/>
+      <c r="H17" s="35"/>
+      <c r="I17" s="40"/>
+      <c r="J17" s="34"/>
+      <c r="K17" s="26"/>
+      <c r="L17" s="34"/>
+      <c r="M17" s="34"/>
+      <c r="N17" s="35"/>
+      <c r="O17" s="40"/>
+      <c r="P17" s="34"/>
+      <c r="Q17" s="34"/>
+      <c r="R17" s="34"/>
+      <c r="S17" s="26"/>
+      <c r="T17" s="35"/>
+      <c r="U17" s="40"/>
+      <c r="V17" s="34"/>
+      <c r="W17" s="34"/>
+      <c r="X17" s="26"/>
+      <c r="Y17" s="34"/>
+      <c r="Z17" s="35"/>
+    </row>
+    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A18" s="32"/>
+      <c r="B18" s="33"/>
+      <c r="C18" s="40"/>
+      <c r="D18" s="34"/>
+      <c r="E18" s="34"/>
+      <c r="F18" s="34"/>
+      <c r="G18" s="34"/>
+      <c r="H18" s="35"/>
+      <c r="I18" s="40"/>
+      <c r="J18" s="34"/>
+      <c r="K18" s="26"/>
+      <c r="L18" s="34"/>
+      <c r="M18" s="34"/>
+      <c r="N18" s="35"/>
+      <c r="O18" s="40"/>
+      <c r="P18" s="34"/>
+      <c r="Q18" s="34"/>
+      <c r="R18" s="34"/>
+      <c r="S18" s="34"/>
+      <c r="T18" s="35"/>
+      <c r="U18" s="40"/>
+      <c r="V18" s="34"/>
+      <c r="W18" s="26"/>
+      <c r="X18" s="26"/>
+      <c r="Y18" s="34"/>
+      <c r="Z18" s="35"/>
+    </row>
+    <row r="19" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="36"/>
+      <c r="B19" s="37"/>
+      <c r="C19" s="41"/>
+      <c r="D19" s="38"/>
+      <c r="E19" s="38"/>
+      <c r="F19" s="38"/>
+      <c r="G19" s="38"/>
+      <c r="H19" s="39"/>
+      <c r="I19" s="41"/>
+      <c r="J19" s="38"/>
+      <c r="K19" s="38"/>
+      <c r="L19" s="38"/>
+      <c r="M19" s="38"/>
+      <c r="N19" s="39"/>
+      <c r="O19" s="41"/>
+      <c r="P19" s="38"/>
+      <c r="Q19" s="38"/>
+      <c r="R19" s="38"/>
+      <c r="S19" s="38"/>
+      <c r="T19" s="39"/>
+      <c r="U19" s="41"/>
+      <c r="V19" s="38"/>
+      <c r="W19" s="38"/>
+      <c r="X19" s="38"/>
+      <c r="Y19" s="38"/>
+      <c r="Z19" s="39"/>
+    </row>
+    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A20" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="29"/>
+      <c r="C20" s="42"/>
+      <c r="D20" s="30"/>
+      <c r="E20" s="30"/>
+      <c r="F20" s="30"/>
+      <c r="G20" s="30"/>
+      <c r="H20" s="31"/>
+      <c r="I20" s="42"/>
+      <c r="J20" s="30"/>
+      <c r="K20" s="30"/>
+      <c r="L20" s="30"/>
+      <c r="M20" s="30"/>
+      <c r="N20" s="31"/>
+      <c r="O20" s="42"/>
+      <c r="P20" s="30"/>
+      <c r="Q20" s="30"/>
+      <c r="R20" s="30"/>
+      <c r="S20" s="30"/>
+      <c r="T20" s="31"/>
+      <c r="U20" s="42"/>
+      <c r="V20" s="30"/>
+      <c r="W20" s="30"/>
+      <c r="X20" s="30"/>
+      <c r="Y20" s="30"/>
+      <c r="Z20" s="31"/>
+    </row>
+    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A21" s="32"/>
+      <c r="B21" s="33"/>
+      <c r="C21" s="40"/>
+      <c r="D21" s="34"/>
+      <c r="E21" s="34"/>
+      <c r="F21" s="34"/>
+      <c r="G21" s="34"/>
+      <c r="H21" s="35"/>
+      <c r="I21" s="40"/>
+      <c r="J21" s="34"/>
+      <c r="K21" s="34"/>
+      <c r="L21" s="34"/>
+      <c r="M21" s="34"/>
+      <c r="N21" s="35"/>
+      <c r="O21" s="40"/>
+      <c r="P21" s="34"/>
+      <c r="Q21" s="34"/>
+      <c r="R21" s="34"/>
+      <c r="S21" s="34"/>
+      <c r="T21" s="35"/>
+      <c r="U21" s="40"/>
+      <c r="V21" s="34"/>
+      <c r="W21" s="34"/>
+      <c r="X21" s="34"/>
+      <c r="Y21" s="34"/>
+      <c r="Z21" s="35"/>
+    </row>
+    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A22" s="32"/>
+      <c r="B22" s="33"/>
+      <c r="C22" s="40"/>
+      <c r="D22" s="34"/>
+      <c r="E22" s="34"/>
+      <c r="F22" s="27"/>
+      <c r="G22" s="34"/>
+      <c r="H22" s="35"/>
+      <c r="I22" s="40"/>
+      <c r="J22" s="34"/>
+      <c r="K22" s="27"/>
+      <c r="L22" s="34"/>
+      <c r="M22" s="34"/>
+      <c r="N22" s="35"/>
+      <c r="O22" s="40"/>
+      <c r="P22" s="34"/>
+      <c r="Q22" s="27"/>
+      <c r="R22" s="27"/>
+      <c r="S22" s="27"/>
+      <c r="T22" s="35"/>
+      <c r="U22" s="40"/>
+      <c r="V22" s="34"/>
+      <c r="W22" s="27"/>
+      <c r="X22" s="27"/>
+      <c r="Y22" s="34"/>
+      <c r="Z22" s="35"/>
+    </row>
+    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A23" s="32"/>
+      <c r="B23" s="33"/>
+      <c r="C23" s="40"/>
+      <c r="D23" s="27"/>
+      <c r="E23" s="27"/>
+      <c r="F23" s="27"/>
+      <c r="G23" s="34"/>
+      <c r="H23" s="35"/>
+      <c r="I23" s="40"/>
+      <c r="J23" s="34"/>
+      <c r="K23" s="27"/>
+      <c r="L23" s="34"/>
+      <c r="M23" s="34"/>
+      <c r="N23" s="35"/>
+      <c r="O23" s="40"/>
+      <c r="P23" s="34"/>
+      <c r="Q23" s="27"/>
+      <c r="R23" s="34"/>
+      <c r="S23" s="34"/>
+      <c r="T23" s="35"/>
+      <c r="U23" s="40"/>
+      <c r="V23" s="34"/>
+      <c r="W23" s="34"/>
+      <c r="X23" s="27"/>
+      <c r="Y23" s="34"/>
+      <c r="Z23" s="35"/>
+    </row>
+    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A24" s="32"/>
+      <c r="B24" s="33"/>
+      <c r="C24" s="40"/>
+      <c r="D24" s="34"/>
+      <c r="E24" s="34"/>
+      <c r="F24" s="34"/>
+      <c r="G24" s="34"/>
+      <c r="H24" s="35"/>
+      <c r="I24" s="40"/>
+      <c r="J24" s="34"/>
+      <c r="K24" s="27"/>
+      <c r="L24" s="27"/>
+      <c r="M24" s="34"/>
+      <c r="N24" s="35"/>
+      <c r="O24" s="40"/>
+      <c r="P24" s="34"/>
+      <c r="Q24" s="34"/>
+      <c r="R24" s="34"/>
+      <c r="S24" s="34"/>
+      <c r="T24" s="35"/>
+      <c r="U24" s="40"/>
+      <c r="V24" s="34"/>
+      <c r="W24" s="34"/>
+      <c r="X24" s="27"/>
+      <c r="Y24" s="34"/>
+      <c r="Z24" s="35"/>
+    </row>
+    <row r="25" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="36"/>
+      <c r="B25" s="37"/>
+      <c r="C25" s="41"/>
+      <c r="D25" s="38"/>
+      <c r="E25" s="38"/>
+      <c r="F25" s="38"/>
+      <c r="G25" s="38"/>
+      <c r="H25" s="39"/>
+      <c r="I25" s="41"/>
+      <c r="J25" s="38"/>
+      <c r="K25" s="38"/>
+      <c r="L25" s="38"/>
+      <c r="M25" s="38"/>
+      <c r="N25" s="39"/>
+      <c r="O25" s="41"/>
+      <c r="P25" s="38"/>
+      <c r="Q25" s="38"/>
+      <c r="R25" s="38"/>
+      <c r="S25" s="38"/>
+      <c r="T25" s="39"/>
+      <c r="U25" s="41"/>
+      <c r="V25" s="38"/>
+      <c r="W25" s="38"/>
+      <c r="X25" s="38"/>
+      <c r="Y25" s="38"/>
+      <c r="Z25" s="39"/>
+    </row>
+    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A26" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="B26" s="29"/>
+      <c r="C26" s="42"/>
+      <c r="D26" s="30"/>
+      <c r="E26" s="30"/>
+      <c r="F26" s="30"/>
+      <c r="G26" s="30"/>
+      <c r="H26" s="31"/>
+      <c r="I26" s="42"/>
+      <c r="J26" s="30"/>
+      <c r="K26" s="30"/>
+      <c r="L26" s="30"/>
+      <c r="M26" s="30"/>
+      <c r="N26" s="31"/>
+      <c r="O26" s="42"/>
+      <c r="P26" s="30"/>
+      <c r="Q26" s="30"/>
+      <c r="R26" s="30"/>
+      <c r="S26" s="30"/>
+      <c r="T26" s="31"/>
+      <c r="U26" s="42"/>
+      <c r="V26" s="30"/>
+      <c r="W26" s="30"/>
+      <c r="X26" s="30"/>
+      <c r="Y26" s="30"/>
+      <c r="Z26" s="31"/>
+    </row>
+    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A27" s="32"/>
+      <c r="B27" s="33"/>
+      <c r="C27" s="40"/>
+      <c r="D27" s="34"/>
+      <c r="E27" s="34"/>
+      <c r="F27" s="34"/>
+      <c r="G27" s="34"/>
+      <c r="H27" s="35"/>
+      <c r="I27" s="40"/>
+      <c r="J27" s="34"/>
+      <c r="K27" s="34"/>
+      <c r="L27" s="34"/>
+      <c r="M27" s="34"/>
+      <c r="N27" s="35"/>
+      <c r="O27" s="40"/>
+      <c r="P27" s="34"/>
+      <c r="Q27" s="34"/>
+      <c r="R27" s="34"/>
+      <c r="S27" s="34"/>
+      <c r="T27" s="35"/>
+      <c r="U27" s="40"/>
+      <c r="V27" s="34"/>
+      <c r="W27" s="34"/>
+      <c r="X27" s="34"/>
+      <c r="Y27" s="34"/>
+      <c r="Z27" s="35"/>
+    </row>
+    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A28" s="32"/>
+      <c r="B28" s="33"/>
+      <c r="C28" s="40"/>
+      <c r="D28" s="34"/>
+      <c r="E28" s="52"/>
+      <c r="F28" s="52"/>
+      <c r="G28" s="34"/>
+      <c r="H28" s="35"/>
+      <c r="I28" s="40"/>
+      <c r="J28" s="34"/>
+      <c r="K28" s="52"/>
+      <c r="L28" s="34"/>
+      <c r="M28" s="34"/>
+      <c r="N28" s="35"/>
+      <c r="O28" s="40"/>
+      <c r="P28" s="34"/>
+      <c r="Q28" s="52"/>
+      <c r="R28" s="52"/>
+      <c r="S28" s="34"/>
+      <c r="T28" s="35"/>
+      <c r="U28" s="40"/>
+      <c r="V28" s="34"/>
+      <c r="W28" s="52"/>
+      <c r="X28" s="34"/>
+      <c r="Y28" s="34"/>
+      <c r="Z28" s="35"/>
+    </row>
+    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A29" s="32"/>
+      <c r="B29" s="33"/>
+      <c r="C29" s="40"/>
+      <c r="D29" s="52"/>
+      <c r="E29" s="52"/>
+      <c r="F29" s="34"/>
+      <c r="G29" s="34"/>
+      <c r="H29" s="35"/>
+      <c r="I29" s="40"/>
+      <c r="J29" s="34"/>
+      <c r="K29" s="52"/>
+      <c r="L29" s="52"/>
+      <c r="M29" s="34"/>
+      <c r="N29" s="35"/>
+      <c r="O29" s="40"/>
+      <c r="P29" s="52"/>
+      <c r="Q29" s="52"/>
+      <c r="R29" s="34"/>
+      <c r="S29" s="34"/>
+      <c r="T29" s="35"/>
+      <c r="U29" s="40"/>
+      <c r="V29" s="34"/>
+      <c r="W29" s="52"/>
+      <c r="X29" s="52"/>
+      <c r="Y29" s="34"/>
+      <c r="Z29" s="35"/>
+    </row>
+    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A30" s="32"/>
+      <c r="B30" s="33"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="34"/>
+      <c r="E30" s="34"/>
+      <c r="F30" s="34"/>
+      <c r="G30" s="34"/>
+      <c r="H30" s="35"/>
+      <c r="I30" s="40"/>
+      <c r="J30" s="34"/>
+      <c r="K30" s="34"/>
+      <c r="L30" s="52"/>
+      <c r="M30" s="34"/>
+      <c r="N30" s="35"/>
+      <c r="O30" s="40"/>
+      <c r="P30" s="34"/>
+      <c r="Q30" s="34"/>
+      <c r="R30" s="34"/>
+      <c r="S30" s="34"/>
+      <c r="T30" s="35"/>
+      <c r="U30" s="40"/>
+      <c r="V30" s="34"/>
+      <c r="W30" s="34"/>
+      <c r="X30" s="52"/>
+      <c r="Y30" s="34"/>
+      <c r="Z30" s="35"/>
+    </row>
+    <row r="31" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="36"/>
+      <c r="B31" s="37"/>
+      <c r="C31" s="41"/>
+      <c r="D31" s="38"/>
+      <c r="E31" s="38"/>
+      <c r="F31" s="38"/>
+      <c r="G31" s="38"/>
+      <c r="H31" s="39"/>
+      <c r="I31" s="41"/>
+      <c r="J31" s="38"/>
+      <c r="K31" s="38"/>
+      <c r="L31" s="38"/>
+      <c r="M31" s="38"/>
+      <c r="N31" s="39"/>
+      <c r="O31" s="41"/>
+      <c r="P31" s="38"/>
+      <c r="Q31" s="38"/>
+      <c r="R31" s="38"/>
+      <c r="S31" s="38"/>
+      <c r="T31" s="39"/>
+      <c r="U31" s="41"/>
+      <c r="V31" s="38"/>
+      <c r="W31" s="38"/>
+      <c r="X31" s="38"/>
+      <c r="Y31" s="38"/>
+      <c r="Z31" s="39"/>
+    </row>
+    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A32" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="B32" s="29"/>
+      <c r="C32" s="42"/>
+      <c r="D32" s="30"/>
+      <c r="E32" s="30"/>
+      <c r="F32" s="30"/>
+      <c r="G32" s="30"/>
+      <c r="H32" s="31"/>
+      <c r="I32" s="42"/>
+      <c r="J32" s="30"/>
+      <c r="K32" s="30"/>
+      <c r="L32" s="30"/>
+      <c r="M32" s="30"/>
+      <c r="N32" s="31"/>
+      <c r="O32" s="42"/>
+      <c r="P32" s="30"/>
+      <c r="Q32" s="30"/>
+      <c r="R32" s="30"/>
+      <c r="S32" s="30"/>
+      <c r="T32" s="31"/>
+      <c r="U32" s="42"/>
+      <c r="V32" s="30"/>
+      <c r="W32" s="30"/>
+      <c r="X32" s="30"/>
+      <c r="Y32" s="30"/>
+      <c r="Z32" s="31"/>
+    </row>
+    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A33" s="32"/>
+      <c r="B33" s="33"/>
+      <c r="C33" s="40"/>
+      <c r="D33" s="34"/>
+      <c r="E33" s="34"/>
+      <c r="F33" s="34"/>
+      <c r="G33" s="34"/>
+      <c r="H33" s="35"/>
+      <c r="I33" s="40"/>
+      <c r="J33" s="34"/>
+      <c r="K33" s="34"/>
+      <c r="L33" s="34"/>
+      <c r="M33" s="34"/>
+      <c r="N33" s="35"/>
+      <c r="O33" s="40"/>
+      <c r="P33" s="34"/>
+      <c r="Q33" s="34"/>
+      <c r="R33" s="34"/>
+      <c r="S33" s="34"/>
+      <c r="T33" s="35"/>
+      <c r="U33" s="40"/>
+      <c r="V33" s="34"/>
+      <c r="W33" s="34"/>
+      <c r="X33" s="34"/>
+      <c r="Y33" s="34"/>
+      <c r="Z33" s="35"/>
+    </row>
+    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A34" s="32"/>
+      <c r="B34" s="33"/>
+      <c r="C34" s="40"/>
+      <c r="D34" s="53"/>
+      <c r="E34" s="53"/>
+      <c r="F34" s="34"/>
+      <c r="G34" s="34"/>
+      <c r="H34" s="35"/>
+      <c r="I34" s="40"/>
+      <c r="J34" s="34"/>
+      <c r="K34" s="34"/>
+      <c r="L34" s="53"/>
+      <c r="M34" s="34"/>
+      <c r="N34" s="35"/>
+      <c r="O34" s="40"/>
+      <c r="P34" s="53"/>
+      <c r="Q34" s="53"/>
+      <c r="R34" s="34"/>
+      <c r="S34" s="34"/>
+      <c r="T34" s="35"/>
+      <c r="U34" s="40"/>
+      <c r="V34" s="34"/>
+      <c r="W34" s="34"/>
+      <c r="X34" s="53"/>
+      <c r="Y34" s="34"/>
+      <c r="Z34" s="35"/>
+    </row>
+    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A35" s="32"/>
+      <c r="B35" s="33"/>
+      <c r="C35" s="40"/>
+      <c r="D35" s="34"/>
+      <c r="E35" s="53"/>
+      <c r="F35" s="53"/>
+      <c r="G35" s="34"/>
+      <c r="H35" s="35"/>
+      <c r="I35" s="40"/>
+      <c r="J35" s="34"/>
+      <c r="K35" s="53"/>
+      <c r="L35" s="53"/>
+      <c r="M35" s="34"/>
+      <c r="N35" s="35"/>
+      <c r="O35" s="40"/>
+      <c r="P35" s="34"/>
+      <c r="Q35" s="53"/>
+      <c r="R35" s="53"/>
+      <c r="S35" s="34"/>
+      <c r="T35" s="35"/>
+      <c r="U35" s="40"/>
+      <c r="V35" s="34"/>
+      <c r="W35" s="53"/>
+      <c r="X35" s="53"/>
+      <c r="Y35" s="34"/>
+      <c r="Z35" s="35"/>
+    </row>
+    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A36" s="32"/>
+      <c r="B36" s="33"/>
+      <c r="C36" s="40"/>
+      <c r="D36" s="34"/>
+      <c r="E36" s="34"/>
+      <c r="F36" s="34"/>
+      <c r="G36" s="34"/>
+      <c r="H36" s="35"/>
+      <c r="I36" s="40"/>
+      <c r="J36" s="34"/>
+      <c r="K36" s="53"/>
+      <c r="L36" s="34"/>
+      <c r="M36" s="34"/>
+      <c r="N36" s="35"/>
+      <c r="O36" s="40"/>
+      <c r="P36" s="34"/>
+      <c r="Q36" s="34"/>
+      <c r="R36" s="34"/>
+      <c r="S36" s="34"/>
+      <c r="T36" s="35"/>
+      <c r="U36" s="40"/>
+      <c r="V36" s="34"/>
+      <c r="W36" s="53"/>
+      <c r="X36" s="34"/>
+      <c r="Y36" s="34"/>
+      <c r="Z36" s="35"/>
+    </row>
+    <row r="37" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="36"/>
+      <c r="B37" s="37"/>
+      <c r="C37" s="41"/>
+      <c r="D37" s="38"/>
+      <c r="E37" s="38"/>
+      <c r="F37" s="38"/>
+      <c r="G37" s="38"/>
+      <c r="H37" s="39"/>
+      <c r="I37" s="41"/>
+      <c r="J37" s="38"/>
+      <c r="K37" s="38"/>
+      <c r="L37" s="38"/>
+      <c r="M37" s="38"/>
+      <c r="N37" s="39"/>
+      <c r="O37" s="41"/>
+      <c r="P37" s="38"/>
+      <c r="Q37" s="38"/>
+      <c r="R37" s="38"/>
+      <c r="S37" s="38"/>
+      <c r="T37" s="39"/>
+      <c r="U37" s="41"/>
+      <c r="V37" s="38"/>
+      <c r="W37" s="38"/>
+      <c r="X37" s="38"/>
+      <c r="Y37" s="38"/>
+      <c r="Z37" s="39"/>
+    </row>
+    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A38" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="B38" s="29"/>
+      <c r="C38" s="42"/>
+      <c r="D38" s="30"/>
+      <c r="E38" s="30"/>
+      <c r="F38" s="30"/>
+      <c r="G38" s="30"/>
+      <c r="H38" s="31"/>
+      <c r="I38" s="42"/>
+      <c r="J38" s="30"/>
+      <c r="K38" s="30"/>
+      <c r="L38" s="30"/>
+      <c r="M38" s="30"/>
+      <c r="N38" s="31"/>
+      <c r="O38" s="42"/>
+      <c r="P38" s="30"/>
+      <c r="Q38" s="30"/>
+      <c r="R38" s="30"/>
+      <c r="S38" s="30"/>
+      <c r="T38" s="31"/>
+      <c r="U38" s="42"/>
+      <c r="V38" s="30"/>
+      <c r="W38" s="30"/>
+      <c r="X38" s="30"/>
+      <c r="Y38" s="30"/>
+      <c r="Z38" s="31"/>
+    </row>
+    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A39" s="32"/>
+      <c r="B39" s="33"/>
+      <c r="C39" s="40"/>
+      <c r="D39" s="34"/>
+      <c r="E39" s="34"/>
+      <c r="F39" s="34"/>
+      <c r="G39" s="34"/>
+      <c r="H39" s="35"/>
+      <c r="I39" s="40"/>
+      <c r="J39" s="34"/>
+      <c r="K39" s="34"/>
+      <c r="L39" s="34"/>
+      <c r="M39" s="34"/>
+      <c r="N39" s="35"/>
+      <c r="O39" s="40"/>
+      <c r="P39" s="34"/>
+      <c r="Q39" s="34"/>
+      <c r="R39" s="34"/>
+      <c r="S39" s="34"/>
+      <c r="T39" s="35"/>
+      <c r="U39" s="40"/>
+      <c r="V39" s="34"/>
+      <c r="W39" s="34"/>
+      <c r="X39" s="34"/>
+      <c r="Y39" s="34"/>
+      <c r="Z39" s="35"/>
+    </row>
+    <row r="40" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A40" s="32"/>
+      <c r="B40" s="33"/>
+      <c r="C40" s="40"/>
+      <c r="D40" s="34"/>
+      <c r="E40" s="54"/>
+      <c r="F40" s="34"/>
+      <c r="G40" s="34"/>
+      <c r="H40" s="35"/>
+      <c r="I40" s="40"/>
+      <c r="J40" s="34"/>
+      <c r="K40" s="54"/>
+      <c r="L40" s="34"/>
+      <c r="M40" s="34"/>
+      <c r="N40" s="35"/>
+      <c r="O40" s="40"/>
+      <c r="P40" s="34"/>
+      <c r="Q40" s="34"/>
+      <c r="R40" s="34"/>
+      <c r="S40" s="34"/>
+      <c r="T40" s="35"/>
+      <c r="U40" s="40"/>
+      <c r="V40" s="34"/>
+      <c r="W40" s="54"/>
+      <c r="X40" s="34"/>
+      <c r="Y40" s="34"/>
+      <c r="Z40" s="35"/>
+    </row>
+    <row r="41" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A41" s="32"/>
+      <c r="B41" s="33"/>
+      <c r="C41" s="40"/>
+      <c r="D41" s="54"/>
+      <c r="E41" s="54"/>
+      <c r="F41" s="54"/>
+      <c r="G41" s="34"/>
+      <c r="H41" s="35"/>
+      <c r="I41" s="40"/>
+      <c r="J41" s="34"/>
+      <c r="K41" s="54"/>
+      <c r="L41" s="54"/>
+      <c r="M41" s="34"/>
+      <c r="N41" s="35"/>
+      <c r="O41" s="40"/>
+      <c r="P41" s="54"/>
+      <c r="Q41" s="54"/>
+      <c r="R41" s="54"/>
+      <c r="S41" s="34"/>
+      <c r="T41" s="35"/>
+      <c r="U41" s="40"/>
+      <c r="V41" s="54"/>
+      <c r="W41" s="54"/>
+      <c r="X41" s="34"/>
+      <c r="Y41" s="34"/>
+      <c r="Z41" s="35"/>
+    </row>
+    <row r="42" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A42" s="32"/>
+      <c r="B42" s="33"/>
+      <c r="C42" s="40"/>
+      <c r="D42" s="34"/>
+      <c r="E42" s="34"/>
+      <c r="F42" s="34"/>
+      <c r="G42" s="34"/>
+      <c r="H42" s="35"/>
+      <c r="I42" s="40"/>
+      <c r="J42" s="34"/>
+      <c r="K42" s="54"/>
+      <c r="L42" s="34"/>
+      <c r="M42" s="34"/>
+      <c r="N42" s="35"/>
+      <c r="O42" s="40"/>
+      <c r="P42" s="34"/>
+      <c r="Q42" s="54"/>
+      <c r="R42" s="34"/>
+      <c r="S42" s="34"/>
+      <c r="T42" s="35"/>
+      <c r="U42" s="40"/>
+      <c r="V42" s="34"/>
+      <c r="W42" s="54"/>
+      <c r="X42" s="34"/>
+      <c r="Y42" s="34"/>
+      <c r="Z42" s="35"/>
+    </row>
+    <row r="43" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="36"/>
+      <c r="B43" s="37"/>
+      <c r="C43" s="41"/>
+      <c r="D43" s="38"/>
+      <c r="E43" s="38"/>
+      <c r="F43" s="38"/>
+      <c r="G43" s="38"/>
+      <c r="H43" s="39"/>
+      <c r="I43" s="41"/>
+      <c r="J43" s="38"/>
+      <c r="K43" s="38"/>
+      <c r="L43" s="38"/>
+      <c r="M43" s="38"/>
+      <c r="N43" s="39"/>
+      <c r="O43" s="41"/>
+      <c r="P43" s="38"/>
+      <c r="Q43" s="38"/>
+      <c r="R43" s="38"/>
+      <c r="S43" s="38"/>
+      <c r="T43" s="39"/>
+      <c r="U43" s="41"/>
+      <c r="V43" s="38"/>
+      <c r="W43" s="38"/>
+      <c r="X43" s="38"/>
+      <c r="Y43" s="38"/>
+      <c r="Z43" s="39"/>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="A14:B19"/>
+    <mergeCell ref="A20:B25"/>
+    <mergeCell ref="A26:B31"/>
+    <mergeCell ref="A32:B37"/>
+    <mergeCell ref="A38:B43"/>
+    <mergeCell ref="C1:H1"/>
+    <mergeCell ref="I1:N1"/>
+    <mergeCell ref="O1:T1"/>
+    <mergeCell ref="U1:Z1"/>
+    <mergeCell ref="A8:B13"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B7"/>
+  </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>